<commit_message>
update plan import code to set standard_plan flag for SHOP market plans
</commit_message>
<xml_diff>
--- a/spec/test_data/plan_data/master_xml/2018/SHOP_MAMaster_Test_Data.xlsx
+++ b/spec/test_data/plan_data/master_xml/2018/SHOP_MAMaster_Test_Data.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishu/healthconnector/enroll/spec/test_data/plan_data/master_xml/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varun/Documents/Ideacrew/enrroll/spec/test_data/plan_data/master_xml/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD93D4F-262C-7044-827A-9C2761BFF1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1360" windowWidth="23100" windowHeight="15480" activeTab="1"/>
+    <workbookView xWindow="5320" yWindow="1360" windowWidth="23100" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2018_QHP" sheetId="1" r:id="rId1"/>
+    <sheet name="SHOP Q1" sheetId="1" r:id="rId1"/>
     <sheet name="2018_QDP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>HMO</t>
   </si>
@@ -129,12 +125,15 @@
   </si>
   <si>
     <t>Rx Formulary Url</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -552,11 +551,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -679,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -717,10 +716,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update plan import code to set standard_plan flag for SHOP market plans (#2008)
Co-authored-by: Jacob Kagon <69021620+jacobkagon@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/spec/test_data/plan_data/master_xml/2018/SHOP_MAMaster_Test_Data.xlsx
+++ b/spec/test_data/plan_data/master_xml/2018/SHOP_MAMaster_Test_Data.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishu/healthconnector/enroll/spec/test_data/plan_data/master_xml/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varun/Documents/Ideacrew/enrroll/spec/test_data/plan_data/master_xml/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD93D4F-262C-7044-827A-9C2761BFF1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="1360" windowWidth="23100" windowHeight="15480" activeTab="1"/>
+    <workbookView xWindow="5320" yWindow="1360" windowWidth="23100" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2018_QHP" sheetId="1" r:id="rId1"/>
+    <sheet name="SHOP Q1" sheetId="1" r:id="rId1"/>
     <sheet name="2018_QDP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,17 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>HMO</t>
   </si>
@@ -129,12 +125,15 @@
   </si>
   <si>
     <t>Rx Formulary Url</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -552,11 +551,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>25</v>
@@ -679,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -717,10 +716,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>